<commit_message>
correction code PS => P01 e0d8c264a3672969b1a0bbd9f27367d5a3092e6f
</commit_message>
<xml_diff>
--- a/sd-corrections-questionnaire/ig/StructureDefinition-ror-questionnaire.xlsx
+++ b/sd-corrections-questionnaire/ig/StructureDefinition-ror-questionnaire.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-28T12:44:22+00:00</t>
+    <t>2024-03-28T13:28:20+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -971,7 +971,7 @@
   <si>
     <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
   &lt;system value="https://mos.esante.gouv.fr/NOS/TRE_R288-TypeProfession/FHIR/TRE-R288-TypeProfession"/&gt;
-  &lt;code value="PS"/&gt;
+  &lt;code value="P01"/&gt;
 &lt;/valueCoding&gt;</t>
   </si>
   <si>

</xml_diff>

<commit_message>
test without binding b28e64c50c6cd61ff7e27503fd99d368a68e0854
</commit_message>
<xml_diff>
--- a/sd-corrections-questionnaire/ig/StructureDefinition-ror-questionnaire.xlsx
+++ b/sd-corrections-questionnaire/ig/StructureDefinition-ror-questionnaire.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3161" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3164" uniqueCount="525">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-28T16:20:19+00:00</t>
+    <t>2024-03-28T17:00:10+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -817,7 +817,7 @@
     <t>Assist in searching for appropriate content.</t>
   </si>
   <si>
-    <t xml:space="preserve">pattern:useContext.code}
+    <t xml:space="preserve">value:useContext.code}
 </t>
   </si>
   <si>
@@ -891,7 +891,10 @@
     <t>extensible</t>
   </si>
   <si>
-    <t>https://interop.esante.gouv.fr/ig/fhir/ror/ValueSet/ror-usage-context-type-vs</t>
+    <t>A code that specifies a type of context being specified by a usage context.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/usage-context-type</t>
   </si>
   <si>
     <t>UsageContext.code</t>
@@ -2016,7 +2019,7 @@
     <col min="25" max="25" width="86.3125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="96.27734375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="25.05859375" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="23.30078125" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="188.67578125" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>
@@ -5277,9 +5280,11 @@
       <c r="X28" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="Y28" s="2"/>
+      <c r="Y28" t="s" s="2">
+        <v>280</v>
+      </c>
       <c r="Z28" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AA28" t="s" s="2">
         <v>80</v>
@@ -5297,7 +5302,7 @@
         <v>80</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>87</v>
@@ -5315,7 +5320,7 @@
         <v>80</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AM28" t="s" s="2">
         <v>80</v>
@@ -5324,15 +5329,15 @@
         <v>80</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5355,13 +5360,13 @@
         <v>88</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -5388,19 +5393,19 @@
         <v>80</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="Z29" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AA29" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AB29" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AC29" s="2"/>
       <c r="AD29" t="s" s="2">
@@ -5410,7 +5415,7 @@
         <v>141</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>87</v>
@@ -5442,13 +5447,13 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C30" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D30" t="s" s="2">
         <v>80</v>
@@ -5470,13 +5475,13 @@
         <v>88</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -5507,7 +5512,7 @@
       </c>
       <c r="Y30" s="2"/>
       <c r="Z30" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AA30" t="s" s="2">
         <v>80</v>
@@ -5525,7 +5530,7 @@
         <v>80</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>87</v>
@@ -5557,13 +5562,13 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="B31" t="s" s="2">
         <v>251</v>
       </c>
       <c r="C31" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D31" t="s" s="2">
         <v>80</v>
@@ -5588,7 +5593,7 @@
         <v>252</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="M31" t="s" s="2">
         <v>254</v>
@@ -5678,7 +5683,7 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B32" t="s" s="2">
         <v>264</v>
@@ -5793,7 +5798,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B33" t="s" s="2">
         <v>269</v>
@@ -5910,7 +5915,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B34" t="s" s="2">
         <v>273</v>
@@ -5956,7 +5961,7 @@
         <v>80</v>
       </c>
       <c r="S34" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="T34" t="s" s="2">
         <v>80</v>
@@ -5973,9 +5978,11 @@
       <c r="X34" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="Y34" s="2"/>
+      <c r="Y34" t="s" s="2">
+        <v>280</v>
+      </c>
       <c r="Z34" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AA34" t="s" s="2">
         <v>80</v>
@@ -5993,7 +6000,7 @@
         <v>80</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>87</v>
@@ -6011,7 +6018,7 @@
         <v>80</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>80</v>
@@ -6020,15 +6027,15 @@
         <v>80</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -6051,13 +6058,13 @@
         <v>88</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -6084,19 +6091,19 @@
         <v>80</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="Z35" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AB35" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AC35" s="2"/>
       <c r="AD35" t="s" s="2">
@@ -6106,7 +6113,7 @@
         <v>141</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>87</v>
@@ -6138,13 +6145,13 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C36" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D36" t="s" s="2">
         <v>80</v>
@@ -6166,13 +6173,13 @@
         <v>88</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M36" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N36" s="2"/>
       <c r="O36" s="2"/>
@@ -6203,7 +6210,7 @@
       </c>
       <c r="Y36" s="2"/>
       <c r="Z36" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="AA36" t="s" s="2">
         <v>80</v>
@@ -6221,7 +6228,7 @@
         <v>80</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>87</v>
@@ -6253,13 +6260,13 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B37" t="s" s="2">
         <v>251</v>
       </c>
       <c r="C37" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D37" t="s" s="2">
         <v>80</v>
@@ -6284,7 +6291,7 @@
         <v>252</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="M37" t="s" s="2">
         <v>254</v>
@@ -6374,7 +6381,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B38" t="s" s="2">
         <v>264</v>
@@ -6489,7 +6496,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="B39" t="s" s="2">
         <v>269</v>
@@ -6606,7 +6613,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B40" t="s" s="2">
         <v>273</v>
@@ -6652,7 +6659,7 @@
         <v>80</v>
       </c>
       <c r="S40" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="T40" t="s" s="2">
         <v>80</v>
@@ -6669,9 +6676,11 @@
       <c r="X40" t="s" s="2">
         <v>279</v>
       </c>
-      <c r="Y40" s="2"/>
+      <c r="Y40" t="s" s="2">
+        <v>280</v>
+      </c>
       <c r="Z40" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AA40" t="s" s="2">
         <v>80</v>
@@ -6689,7 +6698,7 @@
         <v>80</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>87</v>
@@ -6707,7 +6716,7 @@
         <v>80</v>
       </c>
       <c r="AL40" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AM40" t="s" s="2">
         <v>80</v>
@@ -6716,15 +6725,15 @@
         <v>80</v>
       </c>
       <c r="AO40" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6747,13 +6756,13 @@
         <v>88</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -6780,19 +6789,19 @@
         <v>80</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AB41" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AC41" s="2"/>
       <c r="AD41" t="s" s="2">
@@ -6802,7 +6811,7 @@
         <v>141</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>87</v>
@@ -6834,13 +6843,13 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C42" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="D42" t="s" s="2">
         <v>80</v>
@@ -6862,13 +6871,13 @@
         <v>88</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -6899,7 +6908,7 @@
       </c>
       <c r="Y42" s="2"/>
       <c r="Z42" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="AA42" t="s" s="2">
         <v>80</v>
@@ -6917,7 +6926,7 @@
         <v>80</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>87</v>
@@ -6949,10 +6958,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -6975,16 +6984,16 @@
         <v>88</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -7013,10 +7022,10 @@
         <v>279</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="Z43" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AA43" t="s" s="2">
         <v>80</v>
@@ -7034,7 +7043,7 @@
         <v>80</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>78</v>
@@ -7049,7 +7058,7 @@
         <v>100</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>173</v>
@@ -7061,15 +7070,15 @@
         <v>80</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7095,13 +7104,13 @@
         <v>245</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
@@ -7151,7 +7160,7 @@
         <v>80</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>78</v>
@@ -7166,13 +7175,13 @@
         <v>100</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>165</v>
@@ -7183,14 +7192,14 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="E45" s="2"/>
       <c r="F45" t="s" s="2">
@@ -7212,16 +7221,16 @@
         <v>245</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="N45" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="O45" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="P45" t="s" s="2">
         <v>80</v>
@@ -7270,7 +7279,7 @@
         <v>80</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>78</v>
@@ -7285,7 +7294,7 @@
         <v>100</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>173</v>
@@ -7302,10 +7311,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7328,16 +7337,16 @@
         <v>80</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N46" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="O46" s="2"/>
       <c r="P46" t="s" s="2">
@@ -7387,7 +7396,7 @@
         <v>80</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>78</v>
@@ -7402,10 +7411,10 @@
         <v>100</v>
       </c>
       <c r="AK46" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AM46" t="s" s="2">
         <v>80</v>
@@ -7419,10 +7428,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7445,19 +7454,19 @@
         <v>80</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="N47" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="O47" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="P47" t="s" s="2">
         <v>80</v>
@@ -7506,7 +7515,7 @@
         <v>80</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>78</v>
@@ -7521,10 +7530,10 @@
         <v>100</v>
       </c>
       <c r="AK47" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="AM47" t="s" s="2">
         <v>80</v>
@@ -7538,10 +7547,10 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7564,19 +7573,19 @@
         <v>88</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="N48" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="O48" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="P48" t="s" s="2">
         <v>80</v>
@@ -7625,7 +7634,7 @@
         <v>80</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>78</v>
@@ -7637,10 +7646,10 @@
         <v>99</v>
       </c>
       <c r="AJ48" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>173</v>
@@ -7652,15 +7661,15 @@
         <v>165</v>
       </c>
       <c r="AO48" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7686,16 +7695,16 @@
         <v>274</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="N49" t="s" s="2">
         <v>277</v>
       </c>
       <c r="O49" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="P49" t="s" s="2">
         <v>80</v>
@@ -7720,13 +7729,13 @@
         <v>80</v>
       </c>
       <c r="X49" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Y49" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="Z49" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AA49" t="s" s="2">
         <v>80</v>
@@ -7744,7 +7753,7 @@
         <v>80</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>78</v>
@@ -7762,7 +7771,7 @@
         <v>80</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AM49" t="s" s="2">
         <v>80</v>
@@ -7771,15 +7780,15 @@
         <v>80</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
@@ -7802,16 +7811,16 @@
         <v>80</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="O50" s="2"/>
       <c r="P50" t="s" s="2">
@@ -7861,7 +7870,7 @@
         <v>80</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>78</v>
@@ -7870,16 +7879,16 @@
         <v>79</v>
       </c>
       <c r="AI50" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AJ50" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AK50" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AL50" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AM50" t="s" s="2">
         <v>80</v>
@@ -7893,10 +7902,10 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -8008,10 +8017,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8125,14 +8134,14 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" t="s" s="2">
@@ -8154,10 +8163,10 @@
         <v>135</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N53" t="s" s="2">
         <v>138</v>
@@ -8212,7 +8221,7 @@
         <v>80</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>78</v>
@@ -8244,10 +8253,10 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8273,16 +8282,16 @@
         <v>168</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="O54" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="P54" t="s" s="2">
         <v>80</v>
@@ -8331,7 +8340,7 @@
         <v>80</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>87</v>
@@ -8349,7 +8358,7 @@
         <v>80</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AM54" t="s" s="2">
         <v>80</v>
@@ -8363,10 +8372,10 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8392,16 +8401,16 @@
         <v>103</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="O55" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="P55" t="s" s="2">
         <v>80</v>
@@ -8450,7 +8459,7 @@
         <v>80</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>78</v>
@@ -8468,7 +8477,7 @@
         <v>80</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="AM55" t="s" s="2">
         <v>80</v>
@@ -8482,10 +8491,10 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8511,16 +8520,16 @@
         <v>274</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="N56" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="O56" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="P56" t="s" s="2">
         <v>80</v>
@@ -8545,13 +8554,13 @@
         <v>80</v>
       </c>
       <c r="X56" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Y56" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="Z56" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AA56" t="s" s="2">
         <v>80</v>
@@ -8569,7 +8578,7 @@
         <v>80</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>78</v>
@@ -8578,7 +8587,7 @@
         <v>79</v>
       </c>
       <c r="AI56" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AJ56" t="s" s="2">
         <v>100</v>
@@ -8587,7 +8596,7 @@
         <v>80</v>
       </c>
       <c r="AL56" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AM56" t="s" s="2">
         <v>80</v>
@@ -8596,19 +8605,19 @@
         <v>80</v>
       </c>
       <c r="AO56" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E57" s="2"/>
       <c r="F57" t="s" s="2">
@@ -8630,16 +8639,16 @@
         <v>168</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="O57" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="P57" t="s" s="2">
         <v>80</v>
@@ -8688,7 +8697,7 @@
         <v>80</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>78</v>
@@ -8706,7 +8715,7 @@
         <v>80</v>
       </c>
       <c r="AL57" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="AM57" t="s" s="2">
         <v>80</v>
@@ -8720,10 +8729,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8749,13 +8758,13 @@
         <v>168</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" t="s" s="2">
@@ -8805,7 +8814,7 @@
         <v>80</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>78</v>
@@ -8837,10 +8846,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -8866,16 +8875,16 @@
         <v>110</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="O59" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="P59" t="s" s="2">
         <v>80</v>
@@ -8903,10 +8912,10 @@
         <v>199</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="Z59" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="AA59" t="s" s="2">
         <v>80</v>
@@ -8924,7 +8933,7 @@
         <v>80</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>87</v>
@@ -8942,7 +8951,7 @@
         <v>80</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>80</v>
@@ -8956,10 +8965,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -8982,19 +8991,19 @@
         <v>80</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="O60" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="P60" t="s" s="2">
         <v>80</v>
@@ -9043,7 +9052,7 @@
         <v>80</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>78</v>
@@ -9055,13 +9064,13 @@
         <v>99</v>
       </c>
       <c r="AJ60" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AK60" t="s" s="2">
         <v>80</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>80</v>
@@ -9075,10 +9084,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9190,10 +9199,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9307,14 +9316,14 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" t="s" s="2">
@@ -9336,10 +9345,10 @@
         <v>135</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N63" t="s" s="2">
         <v>138</v>
@@ -9394,7 +9403,7 @@
         <v>80</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>78</v>
@@ -9426,10 +9435,10 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9455,13 +9464,13 @@
         <v>168</v>
       </c>
       <c r="L64" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="N64" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="O64" s="2"/>
       <c r="P64" t="s" s="2">
@@ -9511,7 +9520,7 @@
         <v>80</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>87</v>
@@ -9529,7 +9538,7 @@
         <v>80</v>
       </c>
       <c r="AL64" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM64" t="s" s="2">
         <v>80</v>
@@ -9543,10 +9552,10 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9572,13 +9581,13 @@
         <v>110</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="N65" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="O65" s="2"/>
       <c r="P65" t="s" s="2">
@@ -9607,10 +9616,10 @@
         <v>199</v>
       </c>
       <c r="Y65" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="Z65" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AA65" t="s" s="2">
         <v>80</v>
@@ -9628,7 +9637,7 @@
         <v>80</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>87</v>
@@ -9646,7 +9655,7 @@
         <v>80</v>
       </c>
       <c r="AL65" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM65" t="s" s="2">
         <v>80</v>
@@ -9660,10 +9669,10 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -9686,13 +9695,13 @@
         <v>80</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" s="2"/>
@@ -9719,13 +9728,13 @@
         <v>80</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="Z66" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AA66" t="s" s="2">
         <v>80</v>
@@ -9743,7 +9752,7 @@
         <v>80</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>87</v>
@@ -9752,7 +9761,7 @@
         <v>87</v>
       </c>
       <c r="AI66" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AJ66" t="s" s="2">
         <v>100</v>
@@ -9761,7 +9770,7 @@
         <v>80</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>80</v>
@@ -9775,10 +9784,10 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -9804,13 +9813,13 @@
         <v>110</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
@@ -9839,10 +9848,10 @@
         <v>199</v>
       </c>
       <c r="Y67" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="Z67" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="AA67" t="s" s="2">
         <v>80</v>
@@ -9860,7 +9869,7 @@
         <v>80</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>78</v>
@@ -9869,7 +9878,7 @@
         <v>87</v>
       </c>
       <c r="AI67" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="AJ67" t="s" s="2">
         <v>100</v>
@@ -9878,7 +9887,7 @@
         <v>80</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>80</v>
@@ -9892,10 +9901,10 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -9921,20 +9930,20 @@
         <v>206</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="N68" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="O68" s="2"/>
       <c r="P68" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q68" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="R68" t="s" s="2">
         <v>80</v>
@@ -9979,7 +9988,7 @@
         <v>80</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>78</v>
@@ -9988,7 +9997,7 @@
         <v>87</v>
       </c>
       <c r="AI68" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="AJ68" t="s" s="2">
         <v>100</v>
@@ -9997,7 +10006,7 @@
         <v>80</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>80</v>
@@ -10011,10 +10020,10 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -10040,76 +10049,76 @@
         <v>206</v>
       </c>
       <c r="L69" t="s" s="2">
+        <v>464</v>
+      </c>
+      <c r="M69" t="s" s="2">
+        <v>465</v>
+      </c>
+      <c r="N69" t="s" s="2">
+        <v>466</v>
+      </c>
+      <c r="O69" t="s" s="2">
+        <v>467</v>
+      </c>
+      <c r="P69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Q69" t="s" s="2">
+        <v>468</v>
+      </c>
+      <c r="R69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="S69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="T69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="U69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="V69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="W69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="X69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Y69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="Z69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AA69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AB69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AC69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AD69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AE69" t="s" s="2">
+        <v>80</v>
+      </c>
+      <c r="AF69" t="s" s="2">
         <v>463</v>
       </c>
-      <c r="M69" t="s" s="2">
-        <v>464</v>
-      </c>
-      <c r="N69" t="s" s="2">
-        <v>465</v>
-      </c>
-      <c r="O69" t="s" s="2">
-        <v>466</v>
-      </c>
-      <c r="P69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="Q69" t="s" s="2">
-        <v>467</v>
-      </c>
-      <c r="R69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="S69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="T69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="U69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="V69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="W69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="X69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="Y69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="Z69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AA69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AB69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AC69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AD69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AE69" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="AF69" t="s" s="2">
+      <c r="AG69" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AH69" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="AI69" t="s" s="2">
         <v>462</v>
-      </c>
-      <c r="AG69" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AH69" t="s" s="2">
-        <v>87</v>
-      </c>
-      <c r="AI69" t="s" s="2">
-        <v>461</v>
       </c>
       <c r="AJ69" t="s" s="2">
         <v>100</v>
@@ -10118,7 +10127,7 @@
         <v>80</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>80</v>
@@ -10132,10 +10141,10 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10161,16 +10170,16 @@
         <v>206</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="O70" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="P70" t="s" s="2">
         <v>80</v>
@@ -10219,7 +10228,7 @@
         <v>80</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>78</v>
@@ -10228,7 +10237,7 @@
         <v>87</v>
       </c>
       <c r="AI70" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="AJ70" t="s" s="2">
         <v>100</v>
@@ -10237,7 +10246,7 @@
         <v>80</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>80</v>
@@ -10251,10 +10260,10 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10277,16 +10286,16 @@
         <v>80</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="O71" s="2"/>
       <c r="P71" t="s" s="2">
@@ -10336,7 +10345,7 @@
         <v>80</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>78</v>
@@ -10345,7 +10354,7 @@
         <v>87</v>
       </c>
       <c r="AI71" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="AJ71" t="s" s="2">
         <v>100</v>
@@ -10354,7 +10363,7 @@
         <v>80</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM71" t="s" s="2">
         <v>80</v>
@@ -10368,10 +10377,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10394,16 +10403,16 @@
         <v>80</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="N72" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="O72" s="2"/>
       <c r="P72" t="s" s="2">
@@ -10453,7 +10462,7 @@
         <v>80</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>78</v>
@@ -10462,7 +10471,7 @@
         <v>87</v>
       </c>
       <c r="AI72" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AJ72" t="s" s="2">
         <v>100</v>
@@ -10471,7 +10480,7 @@
         <v>80</v>
       </c>
       <c r="AL72" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM72" t="s" s="2">
         <v>80</v>
@@ -10485,10 +10494,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10511,16 +10520,16 @@
         <v>80</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="N73" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="O73" s="2"/>
       <c r="P73" t="s" s="2">
@@ -10570,7 +10579,7 @@
         <v>80</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>78</v>
@@ -10579,7 +10588,7 @@
         <v>79</v>
       </c>
       <c r="AI73" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="AJ73" t="s" s="2">
         <v>100</v>
@@ -10588,7 +10597,7 @@
         <v>80</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM73" t="s" s="2">
         <v>80</v>
@@ -10602,10 +10611,10 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -10717,10 +10726,10 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -10834,14 +10843,14 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" t="s" s="2">
@@ -10863,10 +10872,10 @@
         <v>135</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N76" t="s" s="2">
         <v>138</v>
@@ -10921,7 +10930,7 @@
         <v>80</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>78</v>
@@ -10953,10 +10962,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -10979,16 +10988,16 @@
         <v>80</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="N77" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="O77" s="2"/>
       <c r="P77" t="s" s="2">
@@ -11014,13 +11023,13 @@
         <v>80</v>
       </c>
       <c r="X77" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Y77" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="Z77" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AA77" t="s" s="2">
         <v>80</v>
@@ -11038,7 +11047,7 @@
         <v>80</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>87</v>
@@ -11056,7 +11065,7 @@
         <v>80</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM77" t="s" s="2">
         <v>80</v>
@@ -11070,10 +11079,10 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -11099,20 +11108,20 @@
         <v>206</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="O78" s="2"/>
       <c r="P78" t="s" s="2">
         <v>80</v>
       </c>
       <c r="Q78" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="R78" t="s" s="2">
         <v>80</v>
@@ -11157,7 +11166,7 @@
         <v>80</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>78</v>
@@ -11175,7 +11184,7 @@
         <v>80</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM78" t="s" s="2">
         <v>80</v>
@@ -11189,10 +11198,10 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11215,19 +11224,19 @@
         <v>80</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="O79" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="P79" t="s" s="2">
         <v>80</v>
@@ -11276,7 +11285,7 @@
         <v>80</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>78</v>
@@ -11285,7 +11294,7 @@
         <v>79</v>
       </c>
       <c r="AI79" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="AJ79" t="s" s="2">
         <v>100</v>
@@ -11294,7 +11303,7 @@
         <v>80</v>
       </c>
       <c r="AL79" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM79" t="s" s="2">
         <v>80</v>
@@ -11308,10 +11317,10 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
@@ -11423,10 +11432,10 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11540,14 +11549,14 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E82" s="2"/>
       <c r="F82" t="s" s="2">
@@ -11569,10 +11578,10 @@
         <v>135</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N82" t="s" s="2">
         <v>138</v>
@@ -11627,7 +11636,7 @@
         <v>80</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>78</v>
@@ -11659,10 +11668,10 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
@@ -11685,16 +11694,16 @@
         <v>80</v>
       </c>
       <c r="K83" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="N83" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="O83" s="2"/>
       <c r="P83" t="s" s="2">
@@ -11720,13 +11729,13 @@
         <v>80</v>
       </c>
       <c r="X83" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="Y83" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="Z83" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AA83" t="s" s="2">
         <v>80</v>
@@ -11744,7 +11753,7 @@
         <v>80</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>87</v>
@@ -11762,7 +11771,7 @@
         <v>80</v>
       </c>
       <c r="AL83" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="AM83" t="s" s="2">
         <v>80</v>
@@ -11776,10 +11785,10 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
@@ -11805,16 +11814,16 @@
         <v>81</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="O84" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="P84" t="s" s="2">
         <v>80</v>
@@ -11863,7 +11872,7 @@
         <v>80</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>78</v>
@@ -11872,7 +11881,7 @@
         <v>79</v>
       </c>
       <c r="AI84" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="AJ84" t="s" s="2">
         <v>80</v>
@@ -11881,7 +11890,7 @@
         <v>80</v>
       </c>
       <c r="AL84" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="AM84" t="s" s="2">
         <v>80</v>

</xml_diff>

<commit_message>
add pour questionnaire dans les capability statements 49b2c18256ac6df3513d89d30c97bf9ac7e6e80d
</commit_message>
<xml_diff>
--- a/sd-corrections-questionnaire/ig/StructureDefinition-ror-questionnaire.xlsx
+++ b/sd-corrections-questionnaire/ig/StructureDefinition-ror-questionnaire.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-28T17:14:17+00:00</t>
+    <t>2024-04-02T09:13:36+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -805,7 +805,7 @@
 </t>
   </si>
   <si>
-    <t>Contexte d'usage de la fiche de consignes de saisie de spécifier pour quelle(s) Catégorie(s) d'EG elle est applicable ainsi que pottentiellemnt la spécialité ordinale et la profession</t>
+    <t>Contexte d'usage de la fiche de consignes de saisie de spécifier pour quelle(s) Catégorie(s) d'EG elle est applicable ainsi que potentiellemnt la spécialité ordinale et la profession</t>
   </si>
   <si>
     <t>The content was developed with a focus and intent of supporting the contexts that are listed. These contexts may be general categories (gender, age, ...) or may be references to specific programs (insurance plans, studies, ...) and may be used to assist with indexing and searching for appropriate questionnaire instances.</t>

</xml_diff>

<commit_message>
changement type de slice pour useContext 05cf17f504f5f1beaffd706f57617fb9315a4987
</commit_message>
<xml_diff>
--- a/sd-corrections-questionnaire/ig/StructureDefinition-ror-questionnaire.xlsx
+++ b/sd-corrections-questionnaire/ig/StructureDefinition-ror-questionnaire.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-04-02T10:08:21+00:00</t>
+    <t>2024-04-02T10:29:34+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -817,7 +817,7 @@
     <t>Assist in searching for appropriate content.</t>
   </si>
   <si>
-    <t xml:space="preserve">value:useContext.code}
+    <t xml:space="preserve">pattern:useContext.code}
 </t>
   </si>
   <si>
@@ -2022,7 +2022,7 @@
     <col min="25" max="25" width="86.3125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="96.27734375" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="6.34765625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="23.30078125" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="25.05859375" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="188.67578125" customWidth="true" bestFit="true"/>
     <col min="30" max="30" width="17.21484375" customWidth="true" bestFit="true"/>
     <col min="31" max="31" width="14.4140625" customWidth="true" bestFit="true" hidden="true"/>

</xml_diff>